<commit_message>
Avancement dans le projet...
</commit_message>
<xml_diff>
--- a/uploads/VHU_Syderep.xlsx
+++ b/uploads/VHU_Syderep.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Société</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Précision rubrique</t>
-  </si>
-  <si>
-    <t>Correspond aux centres VHU présents dans le fichier ICPE qui existent dans la BDD</t>
   </si>
   <si>
     <t>CP</t>
@@ -61,7 +58,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,12 +67,6 @@
     </fill>
     <fill>
       <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -105,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -126,7 +117,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,7 +427,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -510,10 +500,8 @@
       <c r="E7" s="3"/>
     </row>
     <row r="18" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H18" s="8"/>
-      <c r="I18" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
@@ -522,6 +510,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Système d'export du fichier VHU_Syderep_copie -> OK
</commit_message>
<xml_diff>
--- a/uploads/VHU_Syderep.xlsx
+++ b/uploads/VHU_Syderep.xlsx
@@ -99,7 +99,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,6 +122,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -430,17 +448,17 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="11" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="14" customWidth="1"/>
     <col min="10" max="10" width="77.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -448,7 +466,7 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -460,57 +478,57 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="4"/>

</xml_diff>